<commit_message>
WS Test Data Changes
</commit_message>
<xml_diff>
--- a/WS_TestData.xlsx
+++ b/WS_TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="15" windowWidth="15270" windowHeight="6210" tabRatio="856" firstSheet="59" activeTab="65"/>
+    <workbookView xWindow="120" yWindow="15" windowWidth="15270" windowHeight="6210" tabRatio="856" firstSheet="59" activeTab="63"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -85,11 +85,11 @@
   </definedNames>
   <calcPr calcId="124519"/>
   <customWorkbookViews>
+    <customWorkbookView name="FedExUser - Personal View" guid="{3EBBAF79-640F-40B1-936A-91016C3870B5}" mergeInterval="0" personalView="1" maximized="1" xWindow="1" yWindow="1" windowWidth="1280" windowHeight="730" tabRatio="856" activeSheetId="3"/>
+    <customWorkbookView name="Amlapure, Basweshwar - Personal View" guid="{E5FAA6DE-C539-4C26-B0D6-51729706E998}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1296" windowHeight="1000" tabRatio="856" activeSheetId="10" showComments="commIndAndComment"/>
+    <customWorkbookView name="Shevtekar, Shubham - Personal View" guid="{80AAF460-4E55-4173-B0EC-8FFFF716C584}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1296" windowHeight="1000" tabRatio="856" activeSheetId="46"/>
+    <customWorkbookView name="Gupta, Sarthika - Personal View" guid="{73682402-F666-4056-BE4D-7C24B9404E6C}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1296" windowHeight="1000" tabRatio="856" activeSheetId="62"/>
     <customWorkbookView name="Singar, Avinash - Personal View" guid="{2AE91CB5-1BF6-456B-808A-28AB556524D4}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1296" windowHeight="1000" tabRatio="856" activeSheetId="20"/>
-    <customWorkbookView name="Gupta, Sarthika - Personal View" guid="{73682402-F666-4056-BE4D-7C24B9404E6C}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1296" windowHeight="1000" tabRatio="856" activeSheetId="62"/>
-    <customWorkbookView name="Shevtekar, Shubham - Personal View" guid="{80AAF460-4E55-4173-B0EC-8FFFF716C584}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1296" windowHeight="1000" tabRatio="856" activeSheetId="46"/>
-    <customWorkbookView name="Amlapure, Basweshwar - Personal View" guid="{E5FAA6DE-C539-4C26-B0D6-51729706E998}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1296" windowHeight="1000" tabRatio="856" activeSheetId="10" showComments="commIndAndComment"/>
-    <customWorkbookView name="FedExUser - Personal View" guid="{3EBBAF79-640F-40B1-936A-91016C3870B5}" mergeInterval="0" personalView="1" maximized="1" xWindow="1" yWindow="1" windowWidth="1280" windowHeight="730" tabRatio="856" activeSheetId="3"/>
   </customWorkbookViews>
 </workbook>
 </file>
@@ -5293,13 +5293,13 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{2AE91CB5-1BF6-456B-808A-28AB556524D4}" showGridLines="0" hiddenColumns="1">
+    <customSheetView guid="{3EBBAF79-640F-40B1-936A-91016C3870B5}" showGridLines="0" hiddenColumns="1">
       <pane xSplit="3" ySplit="4" topLeftCell="H5" activePane="bottomRight" state="frozen"/>
       <selection pane="bottomRight" activeCell="K6" sqref="K6"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{73682402-F666-4056-BE4D-7C24B9404E6C}" showGridLines="0" hiddenColumns="1">
+    <customSheetView guid="{E5FAA6DE-C539-4C26-B0D6-51729706E998}" showGridLines="0" hiddenColumns="1">
       <pane xSplit="3" ySplit="4" topLeftCell="H5" activePane="bottomRight" state="frozen"/>
       <selection pane="bottomRight" activeCell="K6" sqref="K6"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5311,13 +5311,13 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId3"/>
     </customSheetView>
-    <customSheetView guid="{E5FAA6DE-C539-4C26-B0D6-51729706E998}" showGridLines="0" hiddenColumns="1">
+    <customSheetView guid="{73682402-F666-4056-BE4D-7C24B9404E6C}" showGridLines="0" hiddenColumns="1">
       <pane xSplit="3" ySplit="4" topLeftCell="H5" activePane="bottomRight" state="frozen"/>
       <selection pane="bottomRight" activeCell="K6" sqref="K6"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId4"/>
     </customSheetView>
-    <customSheetView guid="{3EBBAF79-640F-40B1-936A-91016C3870B5}" showGridLines="0" hiddenColumns="1">
+    <customSheetView guid="{2AE91CB5-1BF6-456B-808A-28AB556524D4}" showGridLines="0" hiddenColumns="1">
       <pane xSplit="3" ySplit="4" topLeftCell="H5" activePane="bottomRight" state="frozen"/>
       <selection pane="bottomRight" activeCell="K6" sqref="K6"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5325,17 +5325,17 @@
     </customSheetView>
   </customSheetViews>
   <mergeCells count="11">
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="K3:K4"/>
+    <mergeCell ref="L3:L4"/>
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="J3:J4"/>
-    <mergeCell ref="K3:K4"/>
-    <mergeCell ref="L3:L4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId6"/>
@@ -5590,12 +5590,12 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{2AE91CB5-1BF6-456B-808A-28AB556524D4}">
+    <customSheetView guid="{3EBBAF79-640F-40B1-936A-91016C3870B5}">
       <selection activeCell="E2" sqref="E2"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{73682402-F666-4056-BE4D-7C24B9404E6C}">
+    <customSheetView guid="{E5FAA6DE-C539-4C26-B0D6-51729706E998}">
       <selection sqref="A1:F11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
@@ -5605,12 +5605,12 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId3"/>
     </customSheetView>
-    <customSheetView guid="{E5FAA6DE-C539-4C26-B0D6-51729706E998}">
+    <customSheetView guid="{73682402-F666-4056-BE4D-7C24B9404E6C}">
       <selection sqref="A1:F11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId4"/>
     </customSheetView>
-    <customSheetView guid="{3EBBAF79-640F-40B1-936A-91016C3870B5}">
+    <customSheetView guid="{2AE91CB5-1BF6-456B-808A-28AB556524D4}">
       <selection activeCell="E2" sqref="E2"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId5"/>
@@ -5920,12 +5920,12 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{2AE91CB5-1BF6-456B-808A-28AB556524D4}">
+    <customSheetView guid="{3EBBAF79-640F-40B1-936A-91016C3870B5}">
       <selection activeCell="G2" sqref="G2"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{73682402-F666-4056-BE4D-7C24B9404E6C}">
+    <customSheetView guid="{E5FAA6DE-C539-4C26-B0D6-51729706E998}">
       <selection sqref="A1:G13"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
@@ -5935,12 +5935,12 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId3"/>
     </customSheetView>
-    <customSheetView guid="{E5FAA6DE-C539-4C26-B0D6-51729706E998}">
+    <customSheetView guid="{73682402-F666-4056-BE4D-7C24B9404E6C}">
       <selection sqref="A1:G13"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId4"/>
     </customSheetView>
-    <customSheetView guid="{3EBBAF79-640F-40B1-936A-91016C3870B5}">
+    <customSheetView guid="{2AE91CB5-1BF6-456B-808A-28AB556524D4}">
       <selection activeCell="G2" sqref="G2"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId5"/>
@@ -6105,12 +6105,12 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{2AE91CB5-1BF6-456B-808A-28AB556524D4}">
+    <customSheetView guid="{3EBBAF79-640F-40B1-936A-91016C3870B5}">
       <selection activeCell="E2" sqref="E2"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{73682402-F666-4056-BE4D-7C24B9404E6C}">
+    <customSheetView guid="{E5FAA6DE-C539-4C26-B0D6-51729706E998}">
       <selection activeCell="E17" sqref="E17"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
@@ -6120,12 +6120,12 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId3"/>
     </customSheetView>
-    <customSheetView guid="{E5FAA6DE-C539-4C26-B0D6-51729706E998}">
+    <customSheetView guid="{73682402-F666-4056-BE4D-7C24B9404E6C}">
       <selection activeCell="E17" sqref="E17"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId4"/>
     </customSheetView>
-    <customSheetView guid="{3EBBAF79-640F-40B1-936A-91016C3870B5}">
+    <customSheetView guid="{2AE91CB5-1BF6-456B-808A-28AB556524D4}">
       <selection activeCell="E2" sqref="E2"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId5"/>
@@ -6217,11 +6217,11 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{2AE91CB5-1BF6-456B-808A-28AB556524D4}" topLeftCell="C1">
+    <customSheetView guid="{3EBBAF79-640F-40B1-936A-91016C3870B5}" topLeftCell="C1">
       <selection activeCell="E2" sqref="E2:E3"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{73682402-F666-4056-BE4D-7C24B9404E6C}">
+    <customSheetView guid="{E5FAA6DE-C539-4C26-B0D6-51729706E998}">
       <selection sqref="A1:E5"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -6229,11 +6229,11 @@
       <selection sqref="A1:E5"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{E5FAA6DE-C539-4C26-B0D6-51729706E998}">
+    <customSheetView guid="{73682402-F666-4056-BE4D-7C24B9404E6C}">
       <selection sqref="A1:E5"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{3EBBAF79-640F-40B1-936A-91016C3870B5}" topLeftCell="C1">
+    <customSheetView guid="{2AE91CB5-1BF6-456B-808A-28AB556524D4}" topLeftCell="C1">
       <selection activeCell="E2" sqref="E2:E3"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -6328,12 +6328,12 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{2AE91CB5-1BF6-456B-808A-28AB556524D4}">
+    <customSheetView guid="{3EBBAF79-640F-40B1-936A-91016C3870B5}">
       <selection activeCell="C10" sqref="C10"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{73682402-F666-4056-BE4D-7C24B9404E6C}">
+    <customSheetView guid="{E5FAA6DE-C539-4C26-B0D6-51729706E998}">
       <selection activeCell="C13" sqref="C13"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
@@ -6343,12 +6343,12 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId3"/>
     </customSheetView>
-    <customSheetView guid="{E5FAA6DE-C539-4C26-B0D6-51729706E998}">
+    <customSheetView guid="{73682402-F666-4056-BE4D-7C24B9404E6C}">
       <selection activeCell="C13" sqref="C13"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId4"/>
     </customSheetView>
-    <customSheetView guid="{3EBBAF79-640F-40B1-936A-91016C3870B5}">
+    <customSheetView guid="{2AE91CB5-1BF6-456B-808A-28AB556524D4}">
       <selection activeCell="C10" sqref="C10"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId5"/>
@@ -6418,11 +6418,11 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{2AE91CB5-1BF6-456B-808A-28AB556524D4}">
+    <customSheetView guid="{3EBBAF79-640F-40B1-936A-91016C3870B5}">
       <selection activeCell="F32" sqref="F32"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{73682402-F666-4056-BE4D-7C24B9404E6C}">
+    <customSheetView guid="{E5FAA6DE-C539-4C26-B0D6-51729706E998}">
       <selection activeCell="I10" sqref="I10"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -6430,11 +6430,11 @@
       <selection activeCell="I10" sqref="I10"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{E5FAA6DE-C539-4C26-B0D6-51729706E998}">
+    <customSheetView guid="{73682402-F666-4056-BE4D-7C24B9404E6C}">
       <selection activeCell="I10" sqref="I10"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{3EBBAF79-640F-40B1-936A-91016C3870B5}">
+    <customSheetView guid="{2AE91CB5-1BF6-456B-808A-28AB556524D4}">
       <selection activeCell="F32" sqref="F32"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -6899,12 +6899,12 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{2AE91CB5-1BF6-456B-808A-28AB556524D4}" scale="89">
+    <customSheetView guid="{3EBBAF79-640F-40B1-936A-91016C3870B5}" scale="89">
       <selection activeCell="H18" sqref="H18"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{73682402-F666-4056-BE4D-7C24B9404E6C}" scale="89">
+    <customSheetView guid="{E5FAA6DE-C539-4C26-B0D6-51729706E998}" scale="89">
       <selection activeCell="C21" sqref="C21"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
@@ -6914,12 +6914,12 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId3"/>
     </customSheetView>
-    <customSheetView guid="{E5FAA6DE-C539-4C26-B0D6-51729706E998}" scale="89">
+    <customSheetView guid="{73682402-F666-4056-BE4D-7C24B9404E6C}" scale="89">
       <selection activeCell="C21" sqref="C21"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId4"/>
     </customSheetView>
-    <customSheetView guid="{3EBBAF79-640F-40B1-936A-91016C3870B5}" scale="89">
+    <customSheetView guid="{2AE91CB5-1BF6-456B-808A-28AB556524D4}" scale="89">
       <selection activeCell="H18" sqref="H18"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId5"/>
@@ -7400,12 +7400,12 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{2AE91CB5-1BF6-456B-808A-28AB556524D4}">
+    <customSheetView guid="{3EBBAF79-640F-40B1-936A-91016C3870B5}">
       <selection activeCell="E16" sqref="E16:H16"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{73682402-F666-4056-BE4D-7C24B9404E6C}">
+    <customSheetView guid="{E5FAA6DE-C539-4C26-B0D6-51729706E998}">
       <selection activeCell="K13" sqref="K13"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
@@ -7415,12 +7415,12 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId3"/>
     </customSheetView>
-    <customSheetView guid="{E5FAA6DE-C539-4C26-B0D6-51729706E998}">
+    <customSheetView guid="{73682402-F666-4056-BE4D-7C24B9404E6C}">
       <selection activeCell="K13" sqref="K13"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId4"/>
     </customSheetView>
-    <customSheetView guid="{3EBBAF79-640F-40B1-936A-91016C3870B5}">
+    <customSheetView guid="{2AE91CB5-1BF6-456B-808A-28AB556524D4}">
       <selection activeCell="E16" sqref="E16:H16"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId5"/>
@@ -7556,7 +7556,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{2AE91CB5-1BF6-456B-808A-28AB556524D4}">
+    <customSheetView guid="{3EBBAF79-640F-40B1-936A-91016C3870B5}">
       <selection activeCell="E6" sqref="E6"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
@@ -7565,7 +7565,7 @@
       <selection activeCell="O18" sqref="O18"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{3EBBAF79-640F-40B1-936A-91016C3870B5}">
+    <customSheetView guid="{2AE91CB5-1BF6-456B-808A-28AB556524D4}">
       <selection activeCell="E6" sqref="E6"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
@@ -7716,12 +7716,12 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{2AE91CB5-1BF6-456B-808A-28AB556524D4}" scale="90">
+    <customSheetView guid="{3EBBAF79-640F-40B1-936A-91016C3870B5}" scale="90">
       <selection activeCell="F5" sqref="F5"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{73682402-F666-4056-BE4D-7C24B9404E6C}">
+    <customSheetView guid="{E5FAA6DE-C539-4C26-B0D6-51729706E998}">
       <selection activeCell="F15" sqref="F15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
@@ -7731,12 +7731,12 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId3"/>
     </customSheetView>
-    <customSheetView guid="{E5FAA6DE-C539-4C26-B0D6-51729706E998}">
+    <customSheetView guid="{73682402-F666-4056-BE4D-7C24B9404E6C}">
       <selection activeCell="F15" sqref="F15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId4"/>
     </customSheetView>
-    <customSheetView guid="{3EBBAF79-640F-40B1-936A-91016C3870B5}" scale="90">
+    <customSheetView guid="{2AE91CB5-1BF6-456B-808A-28AB556524D4}" scale="90">
       <selection activeCell="F5" sqref="F5"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId5"/>
@@ -8011,13 +8011,13 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{2AE91CB5-1BF6-456B-808A-28AB556524D4}">
+    <customSheetView guid="{3EBBAF79-640F-40B1-936A-91016C3870B5}">
       <selection activeCell="F4" sqref="F4"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{73682402-F666-4056-BE4D-7C24B9404E6C}">
-      <selection activeCell="C6" sqref="C6"/>
+    <customSheetView guid="{E5FAA6DE-C539-4C26-B0D6-51729706E998}" topLeftCell="C1">
+      <selection activeCell="G2" sqref="G2"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
@@ -8026,12 +8026,12 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId3"/>
     </customSheetView>
-    <customSheetView guid="{E5FAA6DE-C539-4C26-B0D6-51729706E998}" topLeftCell="C1">
-      <selection activeCell="G2" sqref="G2"/>
+    <customSheetView guid="{73682402-F666-4056-BE4D-7C24B9404E6C}">
+      <selection activeCell="C6" sqref="C6"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId4"/>
     </customSheetView>
-    <customSheetView guid="{3EBBAF79-640F-40B1-936A-91016C3870B5}">
+    <customSheetView guid="{2AE91CB5-1BF6-456B-808A-28AB556524D4}">
       <selection activeCell="F4" sqref="F4"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId5"/>
@@ -8638,12 +8638,12 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{2AE91CB5-1BF6-456B-808A-28AB556524D4}">
+    <customSheetView guid="{3EBBAF79-640F-40B1-936A-91016C3870B5}">
       <selection activeCell="G2" sqref="G2"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{73682402-F666-4056-BE4D-7C24B9404E6C}">
+    <customSheetView guid="{E5FAA6DE-C539-4C26-B0D6-51729706E998}">
       <selection activeCell="C16" sqref="C16"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
@@ -8653,12 +8653,12 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId3"/>
     </customSheetView>
-    <customSheetView guid="{E5FAA6DE-C539-4C26-B0D6-51729706E998}">
+    <customSheetView guid="{73682402-F666-4056-BE4D-7C24B9404E6C}">
       <selection activeCell="C16" sqref="C16"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId4"/>
     </customSheetView>
-    <customSheetView guid="{3EBBAF79-640F-40B1-936A-91016C3870B5}">
+    <customSheetView guid="{2AE91CB5-1BF6-456B-808A-28AB556524D4}">
       <selection activeCell="G2" sqref="G2"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId5"/>
@@ -9263,12 +9263,12 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{2AE91CB5-1BF6-456B-808A-28AB556524D4}" topLeftCell="C1">
+    <customSheetView guid="{3EBBAF79-640F-40B1-936A-91016C3870B5}" topLeftCell="C1">
       <selection activeCell="K2" sqref="K2"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{73682402-F666-4056-BE4D-7C24B9404E6C}">
+    <customSheetView guid="{E5FAA6DE-C539-4C26-B0D6-51729706E998}">
       <selection activeCell="C30" sqref="C30"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
@@ -9278,12 +9278,12 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId3"/>
     </customSheetView>
-    <customSheetView guid="{E5FAA6DE-C539-4C26-B0D6-51729706E998}">
+    <customSheetView guid="{73682402-F666-4056-BE4D-7C24B9404E6C}">
       <selection activeCell="C30" sqref="C30"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId4"/>
     </customSheetView>
-    <customSheetView guid="{3EBBAF79-640F-40B1-936A-91016C3870B5}" topLeftCell="C1">
+    <customSheetView guid="{2AE91CB5-1BF6-456B-808A-28AB556524D4}" topLeftCell="C1">
       <selection activeCell="K2" sqref="K2"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId5"/>
@@ -9850,12 +9850,12 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{2AE91CB5-1BF6-456B-808A-28AB556524D4}">
+    <customSheetView guid="{3EBBAF79-640F-40B1-936A-91016C3870B5}">
       <selection activeCell="A2" sqref="A2:J24"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{73682402-F666-4056-BE4D-7C24B9404E6C}">
+    <customSheetView guid="{E5FAA6DE-C539-4C26-B0D6-51729706E998}">
       <selection activeCell="A2" sqref="A2:J24"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
@@ -9865,12 +9865,12 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId3"/>
     </customSheetView>
-    <customSheetView guid="{E5FAA6DE-C539-4C26-B0D6-51729706E998}">
+    <customSheetView guid="{73682402-F666-4056-BE4D-7C24B9404E6C}">
       <selection activeCell="A2" sqref="A2:J24"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId4"/>
     </customSheetView>
-    <customSheetView guid="{3EBBAF79-640F-40B1-936A-91016C3870B5}">
+    <customSheetView guid="{2AE91CB5-1BF6-456B-808A-28AB556524D4}">
       <selection activeCell="A2" sqref="A2:J24"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId5"/>
@@ -10097,11 +10097,11 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{2AE91CB5-1BF6-456B-808A-28AB556524D4}">
+    <customSheetView guid="{3EBBAF79-640F-40B1-936A-91016C3870B5}">
       <selection activeCell="C18" sqref="C18"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{73682402-F666-4056-BE4D-7C24B9404E6C}">
+    <customSheetView guid="{E5FAA6DE-C539-4C26-B0D6-51729706E998}">
       <selection activeCell="C18" sqref="C18"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -10110,11 +10110,11 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{E5FAA6DE-C539-4C26-B0D6-51729706E998}">
+    <customSheetView guid="{73682402-F666-4056-BE4D-7C24B9404E6C}">
       <selection activeCell="C18" sqref="C18"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{3EBBAF79-640F-40B1-936A-91016C3870B5}">
+    <customSheetView guid="{2AE91CB5-1BF6-456B-808A-28AB556524D4}">
       <selection activeCell="C18" sqref="C18"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -10425,13 +10425,13 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{2AE91CB5-1BF6-456B-808A-28AB556524D4}">
+    <customSheetView guid="{3EBBAF79-640F-40B1-936A-91016C3870B5}">
       <selection activeCell="E11" sqref="E11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{73682402-F666-4056-BE4D-7C24B9404E6C}" topLeftCell="E1">
-      <selection activeCell="G3" sqref="G3"/>
+    <customSheetView guid="{E5FAA6DE-C539-4C26-B0D6-51729706E998}">
+      <selection activeCell="F7" sqref="F7"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
@@ -10440,12 +10440,12 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId3"/>
     </customSheetView>
-    <customSheetView guid="{E5FAA6DE-C539-4C26-B0D6-51729706E998}">
-      <selection activeCell="F7" sqref="F7"/>
+    <customSheetView guid="{73682402-F666-4056-BE4D-7C24B9404E6C}" topLeftCell="E1">
+      <selection activeCell="G3" sqref="G3"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId4"/>
     </customSheetView>
-    <customSheetView guid="{3EBBAF79-640F-40B1-936A-91016C3870B5}">
+    <customSheetView guid="{2AE91CB5-1BF6-456B-808A-28AB556524D4}">
       <selection activeCell="E11" sqref="E11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId5"/>
@@ -10776,12 +10776,12 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{2AE91CB5-1BF6-456B-808A-28AB556524D4}">
+    <customSheetView guid="{3EBBAF79-640F-40B1-936A-91016C3870B5}">
       <selection activeCell="H39" sqref="H39"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{73682402-F666-4056-BE4D-7C24B9404E6C}">
+    <customSheetView guid="{E5FAA6DE-C539-4C26-B0D6-51729706E998}">
       <selection activeCell="C21" sqref="C21"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
@@ -10791,12 +10791,12 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId3"/>
     </customSheetView>
-    <customSheetView guid="{E5FAA6DE-C539-4C26-B0D6-51729706E998}">
+    <customSheetView guid="{73682402-F666-4056-BE4D-7C24B9404E6C}">
       <selection activeCell="C21" sqref="C21"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId4"/>
     </customSheetView>
-    <customSheetView guid="{3EBBAF79-640F-40B1-936A-91016C3870B5}">
+    <customSheetView guid="{2AE91CB5-1BF6-456B-808A-28AB556524D4}">
       <selection activeCell="H39" sqref="H39"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId5"/>
@@ -10947,12 +10947,12 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{2AE91CB5-1BF6-456B-808A-28AB556524D4}">
+    <customSheetView guid="{3EBBAF79-640F-40B1-936A-91016C3870B5}">
       <selection activeCell="C6" sqref="C6"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{73682402-F666-4056-BE4D-7C24B9404E6C}">
+    <customSheetView guid="{E5FAA6DE-C539-4C26-B0D6-51729706E998}">
       <selection activeCell="C14" sqref="C14"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
@@ -10962,12 +10962,12 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId3"/>
     </customSheetView>
-    <customSheetView guid="{E5FAA6DE-C539-4C26-B0D6-51729706E998}">
+    <customSheetView guid="{73682402-F666-4056-BE4D-7C24B9404E6C}">
       <selection activeCell="C14" sqref="C14"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId4"/>
     </customSheetView>
-    <customSheetView guid="{3EBBAF79-640F-40B1-936A-91016C3870B5}">
+    <customSheetView guid="{2AE91CB5-1BF6-456B-808A-28AB556524D4}">
       <selection activeCell="C6" sqref="C6"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId5"/>
@@ -11086,11 +11086,11 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{2AE91CB5-1BF6-456B-808A-28AB556524D4}">
+    <customSheetView guid="{3EBBAF79-640F-40B1-936A-91016C3870B5}">
       <selection activeCell="C4" sqref="C4"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{73682402-F666-4056-BE4D-7C24B9404E6C}">
+    <customSheetView guid="{E5FAA6DE-C539-4C26-B0D6-51729706E998}">
       <selection sqref="A1:E6"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -11098,11 +11098,11 @@
       <selection sqref="A1:E6"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{E5FAA6DE-C539-4C26-B0D6-51729706E998}">
+    <customSheetView guid="{73682402-F666-4056-BE4D-7C24B9404E6C}">
       <selection sqref="A1:E6"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{3EBBAF79-640F-40B1-936A-91016C3870B5}">
+    <customSheetView guid="{2AE91CB5-1BF6-456B-808A-28AB556524D4}">
       <selection activeCell="C4" sqref="C4"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -11747,11 +11747,11 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{2AE91CB5-1BF6-456B-808A-28AB556524D4}" topLeftCell="D1">
+    <customSheetView guid="{3EBBAF79-640F-40B1-936A-91016C3870B5}" topLeftCell="D1">
       <selection activeCell="F2" sqref="F2"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{73682402-F666-4056-BE4D-7C24B9404E6C}">
+    <customSheetView guid="{E5FAA6DE-C539-4C26-B0D6-51729706E998}">
       <selection activeCell="E12" sqref="E12"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -11759,11 +11759,11 @@
       <selection activeCell="E12" sqref="E12"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{E5FAA6DE-C539-4C26-B0D6-51729706E998}">
+    <customSheetView guid="{73682402-F666-4056-BE4D-7C24B9404E6C}">
       <selection activeCell="E12" sqref="E12"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{3EBBAF79-640F-40B1-936A-91016C3870B5}" topLeftCell="D1">
+    <customSheetView guid="{2AE91CB5-1BF6-456B-808A-28AB556524D4}" topLeftCell="D1">
       <selection activeCell="F2" sqref="F2"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -12408,11 +12408,11 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{2AE91CB5-1BF6-456B-808A-28AB556524D4}">
+    <customSheetView guid="{3EBBAF79-640F-40B1-936A-91016C3870B5}">
       <selection activeCell="A2" sqref="A2:J27"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{73682402-F666-4056-BE4D-7C24B9404E6C}">
+    <customSheetView guid="{E5FAA6DE-C539-4C26-B0D6-51729706E998}">
       <selection sqref="A1:J27"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -12420,11 +12420,11 @@
       <selection sqref="A1:J27"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{E5FAA6DE-C539-4C26-B0D6-51729706E998}">
+    <customSheetView guid="{73682402-F666-4056-BE4D-7C24B9404E6C}">
       <selection sqref="A1:J27"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{3EBBAF79-640F-40B1-936A-91016C3870B5}">
+    <customSheetView guid="{2AE91CB5-1BF6-456B-808A-28AB556524D4}">
       <selection activeCell="A2" sqref="A2:J27"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -12543,23 +12543,23 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{2AE91CB5-1BF6-456B-808A-28AB556524D4}">
+    <customSheetView guid="{3EBBAF79-640F-40B1-936A-91016C3870B5}">
       <selection activeCell="E7" sqref="E7"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{E5FAA6DE-C539-4C26-B0D6-51729706E998}">
+      <selection activeCell="E3" sqref="E3"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{80AAF460-4E55-4173-B0EC-8FFFF716C584}">
+      <selection activeCell="C6" sqref="C6"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
     <customSheetView guid="{73682402-F666-4056-BE4D-7C24B9404E6C}">
       <selection activeCell="C6" sqref="C6"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{80AAF460-4E55-4173-B0EC-8FFFF716C584}">
-      <selection activeCell="C6" sqref="C6"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{E5FAA6DE-C539-4C26-B0D6-51729706E998}">
-      <selection activeCell="E3" sqref="E3"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{3EBBAF79-640F-40B1-936A-91016C3870B5}">
+    <customSheetView guid="{2AE91CB5-1BF6-456B-808A-28AB556524D4}">
       <selection activeCell="E7" sqref="E7"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -13145,12 +13145,12 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{2AE91CB5-1BF6-456B-808A-28AB556524D4}">
+    <customSheetView guid="{3EBBAF79-640F-40B1-936A-91016C3870B5}">
       <selection activeCell="A2" sqref="A2:J25"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{73682402-F666-4056-BE4D-7C24B9404E6C}">
+    <customSheetView guid="{E5FAA6DE-C539-4C26-B0D6-51729706E998}">
       <selection activeCell="A2" sqref="A2:J25"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
@@ -13160,12 +13160,12 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId3"/>
     </customSheetView>
-    <customSheetView guid="{E5FAA6DE-C539-4C26-B0D6-51729706E998}">
+    <customSheetView guid="{73682402-F666-4056-BE4D-7C24B9404E6C}">
       <selection activeCell="A2" sqref="A2:J25"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId4"/>
     </customSheetView>
-    <customSheetView guid="{3EBBAF79-640F-40B1-936A-91016C3870B5}">
+    <customSheetView guid="{2AE91CB5-1BF6-456B-808A-28AB556524D4}">
       <selection activeCell="A2" sqref="A2:J25"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId5"/>
@@ -13399,11 +13399,11 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{2AE91CB5-1BF6-456B-808A-28AB556524D4}" topLeftCell="B1">
+    <customSheetView guid="{3EBBAF79-640F-40B1-936A-91016C3870B5}" topLeftCell="B1">
       <selection activeCell="C7" sqref="C7"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{73682402-F666-4056-BE4D-7C24B9404E6C}" topLeftCell="E1">
+    <customSheetView guid="{E5FAA6DE-C539-4C26-B0D6-51729706E998}" topLeftCell="E1">
       <selection activeCell="C7" sqref="C7"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -13411,11 +13411,11 @@
       <selection activeCell="F9" sqref="F9"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{E5FAA6DE-C539-4C26-B0D6-51729706E998}" topLeftCell="E1">
+    <customSheetView guid="{73682402-F666-4056-BE4D-7C24B9404E6C}" topLeftCell="E1">
       <selection activeCell="C7" sqref="C7"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{3EBBAF79-640F-40B1-936A-91016C3870B5}" topLeftCell="B1">
+    <customSheetView guid="{2AE91CB5-1BF6-456B-808A-28AB556524D4}" topLeftCell="B1">
       <selection activeCell="C7" sqref="C7"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -13520,11 +13520,11 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{2AE91CB5-1BF6-456B-808A-28AB556524D4}">
+    <customSheetView guid="{3EBBAF79-640F-40B1-936A-91016C3870B5}">
       <selection activeCell="A2" sqref="A2:XFD5"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{73682402-F666-4056-BE4D-7C24B9404E6C}">
+    <customSheetView guid="{E5FAA6DE-C539-4C26-B0D6-51729706E998}">
       <selection activeCell="B1" sqref="B1:B1048576"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -13532,11 +13532,11 @@
       <selection activeCell="B1" sqref="B1:B1048576"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{E5FAA6DE-C539-4C26-B0D6-51729706E998}">
+    <customSheetView guid="{73682402-F666-4056-BE4D-7C24B9404E6C}">
       <selection activeCell="B1" sqref="B1:B1048576"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{3EBBAF79-640F-40B1-936A-91016C3870B5}">
+    <customSheetView guid="{2AE91CB5-1BF6-456B-808A-28AB556524D4}">
       <selection activeCell="A2" sqref="A2:XFD5"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -13617,7 +13617,15 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{2AE91CB5-1BF6-456B-808A-28AB556524D4}">
+    <customSheetView guid="{3EBBAF79-640F-40B1-936A-91016C3870B5}">
+      <selection activeCell="C13" sqref="C13"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{E5FAA6DE-C539-4C26-B0D6-51729706E998}">
+      <selection activeCell="C13" sqref="C13"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{80AAF460-4E55-4173-B0EC-8FFFF716C584}">
       <selection activeCell="C13" sqref="C13"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -13625,15 +13633,7 @@
       <selection activeCell="C13" sqref="C13"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{80AAF460-4E55-4173-B0EC-8FFFF716C584}">
-      <selection activeCell="C13" sqref="C13"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{E5FAA6DE-C539-4C26-B0D6-51729706E998}">
-      <selection activeCell="C13" sqref="C13"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{3EBBAF79-640F-40B1-936A-91016C3870B5}">
+    <customSheetView guid="{2AE91CB5-1BF6-456B-808A-28AB556524D4}">
       <selection activeCell="C13" sqref="C13"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -13715,7 +13715,15 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{2AE91CB5-1BF6-456B-808A-28AB556524D4}">
+    <customSheetView guid="{3EBBAF79-640F-40B1-936A-91016C3870B5}">
+      <selection activeCell="C4" sqref="C4"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{E5FAA6DE-C539-4C26-B0D6-51729706E998}">
+      <selection activeCell="C10" sqref="C10"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{80AAF460-4E55-4173-B0EC-8FFFF716C584}">
       <selection activeCell="C4" sqref="C4"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -13723,15 +13731,7 @@
       <selection activeCell="C10" sqref="C10"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{80AAF460-4E55-4173-B0EC-8FFFF716C584}">
-      <selection activeCell="C4" sqref="C4"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{E5FAA6DE-C539-4C26-B0D6-51729706E998}">
-      <selection activeCell="C10" sqref="C10"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{3EBBAF79-640F-40B1-936A-91016C3870B5}">
+    <customSheetView guid="{2AE91CB5-1BF6-456B-808A-28AB556524D4}">
       <selection activeCell="C4" sqref="C4"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -32897,11 +32897,11 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{2AE91CB5-1BF6-456B-808A-28AB556524D4}">
+    <customSheetView guid="{3EBBAF79-640F-40B1-936A-91016C3870B5}">
       <selection activeCell="D41" sqref="D41"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{73682402-F666-4056-BE4D-7C24B9404E6C}">
+    <customSheetView guid="{E5FAA6DE-C539-4C26-B0D6-51729706E998}">
       <selection activeCell="C11" sqref="C11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -32909,11 +32909,11 @@
       <selection activeCell="C11" sqref="C11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{E5FAA6DE-C539-4C26-B0D6-51729706E998}">
+    <customSheetView guid="{73682402-F666-4056-BE4D-7C24B9404E6C}">
       <selection activeCell="C11" sqref="C11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{3EBBAF79-640F-40B1-936A-91016C3870B5}">
+    <customSheetView guid="{2AE91CB5-1BF6-456B-808A-28AB556524D4}">
       <selection activeCell="D41" sqref="D41"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -33610,13 +33610,13 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{2AE91CB5-1BF6-456B-808A-28AB556524D4}" topLeftCell="B1">
+    <customSheetView guid="{3EBBAF79-640F-40B1-936A-91016C3870B5}" topLeftCell="B1">
       <selection activeCell="F2" sqref="F2"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{73682402-F666-4056-BE4D-7C24B9404E6C}">
-      <selection sqref="A1:G1"/>
+    <customSheetView guid="{E5FAA6DE-C539-4C26-B0D6-51729706E998}">
+      <selection activeCell="F2" sqref="F2"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
@@ -33625,12 +33625,12 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId3"/>
     </customSheetView>
-    <customSheetView guid="{E5FAA6DE-C539-4C26-B0D6-51729706E998}">
-      <selection activeCell="F2" sqref="F2"/>
+    <customSheetView guid="{73682402-F666-4056-BE4D-7C24B9404E6C}">
+      <selection sqref="A1:G1"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId4"/>
     </customSheetView>
-    <customSheetView guid="{3EBBAF79-640F-40B1-936A-91016C3870B5}" topLeftCell="B1">
+    <customSheetView guid="{2AE91CB5-1BF6-456B-808A-28AB556524D4}" topLeftCell="B1">
       <selection activeCell="F2" sqref="F2"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId5"/>
@@ -36540,13 +36540,13 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{2AE91CB5-1BF6-456B-808A-28AB556524D4}">
+    <customSheetView guid="{3EBBAF79-640F-40B1-936A-91016C3870B5}">
       <selection activeCell="C5" sqref="C5"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{73682402-F666-4056-BE4D-7C24B9404E6C}">
-      <selection activeCell="C29" sqref="C29"/>
+    <customSheetView guid="{E5FAA6DE-C539-4C26-B0D6-51729706E998}">
+      <selection activeCell="E3" sqref="E3"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
@@ -36555,12 +36555,12 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId3"/>
     </customSheetView>
-    <customSheetView guid="{E5FAA6DE-C539-4C26-B0D6-51729706E998}">
-      <selection activeCell="E3" sqref="E3"/>
+    <customSheetView guid="{73682402-F666-4056-BE4D-7C24B9404E6C}">
+      <selection activeCell="C29" sqref="C29"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId4"/>
     </customSheetView>
-    <customSheetView guid="{3EBBAF79-640F-40B1-936A-91016C3870B5}">
+    <customSheetView guid="{2AE91CB5-1BF6-456B-808A-28AB556524D4}">
       <selection activeCell="C5" sqref="C5"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId5"/>
@@ -46092,12 +46092,12 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{2AE91CB5-1BF6-456B-808A-28AB556524D4}">
+    <customSheetView guid="{3EBBAF79-640F-40B1-936A-91016C3870B5}">
       <selection activeCell="F2" sqref="F2"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{73682402-F666-4056-BE4D-7C24B9404E6C}">
+    <customSheetView guid="{E5FAA6DE-C539-4C26-B0D6-51729706E998}">
       <selection activeCell="C9" sqref="C9"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
@@ -46107,12 +46107,12 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId3"/>
     </customSheetView>
-    <customSheetView guid="{E5FAA6DE-C539-4C26-B0D6-51729706E998}">
+    <customSheetView guid="{73682402-F666-4056-BE4D-7C24B9404E6C}">
       <selection activeCell="C9" sqref="C9"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId4"/>
     </customSheetView>
-    <customSheetView guid="{3EBBAF79-640F-40B1-936A-91016C3870B5}">
+    <customSheetView guid="{2AE91CB5-1BF6-456B-808A-28AB556524D4}">
       <selection activeCell="F2" sqref="F2"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId5"/>
@@ -47879,8 +47879,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:O32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5:H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1"/>
@@ -49469,7 +49469,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -50215,12 +50215,12 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{2AE91CB5-1BF6-456B-808A-28AB556524D4}">
+    <customSheetView guid="{3EBBAF79-640F-40B1-936A-91016C3870B5}">
       <selection activeCell="F2" sqref="F2"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{73682402-F666-4056-BE4D-7C24B9404E6C}">
+    <customSheetView guid="{E5FAA6DE-C539-4C26-B0D6-51729706E998}">
       <selection activeCell="C5" sqref="C5"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
@@ -50230,12 +50230,12 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId3"/>
     </customSheetView>
-    <customSheetView guid="{E5FAA6DE-C539-4C26-B0D6-51729706E998}">
+    <customSheetView guid="{73682402-F666-4056-BE4D-7C24B9404E6C}">
       <selection activeCell="C5" sqref="C5"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId4"/>
     </customSheetView>
-    <customSheetView guid="{3EBBAF79-640F-40B1-936A-91016C3870B5}">
+    <customSheetView guid="{2AE91CB5-1BF6-456B-808A-28AB556524D4}">
       <selection activeCell="F2" sqref="F2"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId5"/>
@@ -50372,12 +50372,12 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{2AE91CB5-1BF6-456B-808A-28AB556524D4}">
+    <customSheetView guid="{3EBBAF79-640F-40B1-936A-91016C3870B5}">
       <selection activeCell="E3" sqref="E3"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{73682402-F666-4056-BE4D-7C24B9404E6C}">
+    <customSheetView guid="{E5FAA6DE-C539-4C26-B0D6-51729706E998}">
       <selection sqref="A1:G1"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
@@ -50387,12 +50387,12 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId3"/>
     </customSheetView>
-    <customSheetView guid="{E5FAA6DE-C539-4C26-B0D6-51729706E998}">
+    <customSheetView guid="{73682402-F666-4056-BE4D-7C24B9404E6C}">
       <selection sqref="A1:G1"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId4"/>
     </customSheetView>
-    <customSheetView guid="{3EBBAF79-640F-40B1-936A-91016C3870B5}">
+    <customSheetView guid="{2AE91CB5-1BF6-456B-808A-28AB556524D4}">
       <selection activeCell="E3" sqref="E3"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId5"/>
@@ -50559,11 +50559,11 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{2AE91CB5-1BF6-456B-808A-28AB556524D4}">
+    <customSheetView guid="{3EBBAF79-640F-40B1-936A-91016C3870B5}">
       <selection activeCell="C5" sqref="C5"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{73682402-F666-4056-BE4D-7C24B9404E6C}">
+    <customSheetView guid="{E5FAA6DE-C539-4C26-B0D6-51729706E998}">
       <selection activeCell="D18" sqref="D18"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -50571,11 +50571,11 @@
       <selection activeCell="D18" sqref="D18"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{E5FAA6DE-C539-4C26-B0D6-51729706E998}">
+    <customSheetView guid="{73682402-F666-4056-BE4D-7C24B9404E6C}">
       <selection activeCell="D18" sqref="D18"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{3EBBAF79-640F-40B1-936A-91016C3870B5}">
+    <customSheetView guid="{2AE91CB5-1BF6-456B-808A-28AB556524D4}">
       <selection activeCell="C5" sqref="C5"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>

</xml_diff>